<commit_message>
Updated all simulations with semi-realistic values
Finalized initial SolidWorks leg model.
Took leg properties and placed them in MATLAB dynamic simulation to
determine required torques and forces.
Took leg geometry and MATLAB output into ANSYS and performed a worst
case failure analysis with immobile joints.
</commit_message>
<xml_diff>
--- a/Software/Agile Controls Simulation/ParameterConfig.xlsx
+++ b/Software/Agile Controls Simulation/ParameterConfig.xlsx
@@ -44,12 +44,6 @@
     <t>Shank CG (from knee) [m]</t>
   </si>
   <si>
-    <t>Shank Moment [m4]</t>
-  </si>
-  <si>
-    <t>Thigh Moment [m4]</t>
-  </si>
-  <si>
     <t>Thigh Distance [cm]</t>
   </si>
   <si>
@@ -60,6 +54,12 @@
   </si>
   <si>
     <t>Body CG [m from front]</t>
+  </si>
+  <si>
+    <t>Thigh Inertia [m4]</t>
+  </si>
+  <si>
+    <t>Shank Inertia [m4]</t>
   </si>
 </sst>
 </file>
@@ -588,34 +588,35 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4">
-        <v>0.25</v>
+        <f>B2/2</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>43.3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6">
-        <v>2.562E-3</v>
+        <v>6.7929000000000004E-4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -623,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -631,23 +632,23 @@
         <v>2</v>
       </c>
       <c r="B7" s="4">
-        <v>0.96</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6">
-        <v>2.24E-4</v>
+        <v>5.1042000000000004E-4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,7 +656,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6">
-        <v>6.0999999999999999E-2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -663,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="4">
-        <v>0.93</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>